<commit_message>
Alter DBN, update CPTs
</commit_message>
<xml_diff>
--- a/CPTs.xlsx
+++ b/CPTs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rylan\Desktop\School\3Year\COSC329\329-Learning-Calendar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Logan\Desktop\COSC 329\Project\329-Learning-Calendar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDDD2FC-7550-46D8-9F4B-86A524157DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45EC84AD-EE04-4218-9D57-8112C6D005EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-8235" windowWidth="16440" windowHeight="28440" xr2:uid="{4FD7F259-FAFA-4789-A3F8-7C8F0A1F6558}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4FD7F259-FAFA-4789-A3F8-7C8F0A1F6558}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="42">
   <si>
     <t>EventImportance</t>
   </si>
@@ -127,6 +127,39 @@
   </si>
   <si>
     <t>Pr(Urgent|Urgent (t-1) )</t>
+  </si>
+  <si>
+    <t>Urgency</t>
+  </si>
+  <si>
+    <t>Busyness</t>
+  </si>
+  <si>
+    <t>CheckedCalendarFrequency</t>
+  </si>
+  <si>
+    <t>Not</t>
+  </si>
+  <si>
+    <t>Busy</t>
+  </si>
+  <si>
+    <t>WithinMonth</t>
+  </si>
+  <si>
+    <t>WithinWeek</t>
+  </si>
+  <si>
+    <t>WithinDay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not </t>
+  </si>
+  <si>
+    <t>noT</t>
+  </si>
+  <si>
+    <t>Very</t>
   </si>
 </sst>
 </file>
@@ -156,7 +189,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,8 +214,20 @@
         <bgColor theme="8" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -266,11 +311,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -278,6 +336,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -296,8 +356,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A3538EFA-96AB-40ED-BC69-DD1D3EEB1D38}" name="Table1" displayName="Table1" ref="A21:B22" totalsRowShown="0">
-  <autoFilter ref="A21:B22" xr:uid="{A3538EFA-96AB-40ED-BC69-DD1D3EEB1D38}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A3538EFA-96AB-40ED-BC69-DD1D3EEB1D38}" name="Table1" displayName="Table1" ref="D21:E22" totalsRowShown="0">
+  <autoFilter ref="D21:E22" xr:uid="{A3538EFA-96AB-40ED-BC69-DD1D3EEB1D38}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{7110FBC9-9E40-49FC-871A-F08C5D9FE788}" name="NeedReminder = False"/>
     <tableColumn id="2" xr3:uid="{F8B689E5-AC8A-4F44-ABEA-B8AF4AC8D64A}" name="NeedReminder = True"/>
@@ -333,8 +393,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A3A416B5-9151-4FD9-8677-22365280045F}" name="Table6" displayName="Table6" ref="A35:C37" totalsRowShown="0">
-  <autoFilter ref="A35:C37" xr:uid="{A3A416B5-9151-4FD9-8677-22365280045F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A3A416B5-9151-4FD9-8677-22365280045F}" name="Table6" displayName="Table6" ref="A70:C72" totalsRowShown="0">
+  <autoFilter ref="A70:C72" xr:uid="{A3A416B5-9151-4FD9-8677-22365280045F}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{972A3304-3633-4EC8-94C1-43B9B2DCB076}" name="Preferences:"/>
     <tableColumn id="2" xr3:uid="{C4B907E5-3F49-40E5-8D85-D8CAA37853D7}" name="Pr(~WantReminder|NeedReminder)"/>
@@ -356,8 +416,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{41948802-5E6F-4D5B-B768-89661C1A722E}" name="Table69" displayName="Table69" ref="A30:D32" totalsRowShown="0">
-  <autoFilter ref="A30:D32" xr:uid="{41948802-5E6F-4D5B-B768-89661C1A722E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{41948802-5E6F-4D5B-B768-89661C1A722E}" name="Table69" displayName="Table69" ref="A65:D67" totalsRowShown="0">
+  <autoFilter ref="A65:D67" xr:uid="{41948802-5E6F-4D5B-B768-89661C1A722E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{2ACB6FC3-D65B-4A5C-B180-9330927FFBF5}" name="Busyness:"/>
     <tableColumn id="2" xr3:uid="{8D9E8C97-7B87-49B1-9718-B12757BCEE3B}" name="Pr(NotBusy|NeedReminder)"/>
@@ -369,8 +429,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{430F4603-BB98-49AB-9C6E-A709BA25E0BB}" name="Table610" displayName="Table610" ref="A40:D42" totalsRowShown="0">
-  <autoFilter ref="A40:D42" xr:uid="{430F4603-BB98-49AB-9C6E-A709BA25E0BB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{430F4603-BB98-49AB-9C6E-A709BA25E0BB}" name="Table610" displayName="Table610" ref="A75:D77" totalsRowShown="0">
+  <autoFilter ref="A75:D77" xr:uid="{430F4603-BB98-49AB-9C6E-A709BA25E0BB}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{88FC3D16-8DEA-416C-83A8-91C4B4BD8A49}" name="CheckedCalendarRecently:"/>
     <tableColumn id="2" xr3:uid="{99D7C84C-7F46-416E-82B2-FC32603E2610}" name="Pr(WithinMonth|NeedReminder)"/>
@@ -378,6 +438,17 @@
     <tableColumn id="4" xr3:uid="{DC03569F-C56E-471E-9971-BC0DB78E91D2}" name="Pr(WithinDay|NeedReminder)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BB536D8A-FC7A-4256-8B80-39CE50AA9B9C}" name="Table15" displayName="Table15" ref="B21:C30" totalsRowShown="0">
+  <autoFilter ref="B21:C30" xr:uid="{BB536D8A-FC7A-4256-8B80-39CE50AA9B9C}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{366E0F95-13BA-436C-9A52-CDFC7E3E6053}" name="Busyness"/>
+    <tableColumn id="2" xr3:uid="{A4AB0B0D-C9D3-439C-9202-89885F20C2FD}" name="CheckedCalendarFrequency"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -678,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F16022FB-2605-4D33-9734-5034D9D67958}">
-  <dimension ref="A2:D42"/>
+  <dimension ref="A2:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,7 +761,7 @@
     <col min="2" max="2" width="39.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -800,7 +871,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -814,7 +885,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -828,169 +899,368 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
         <v>5</v>
       </c>
-      <c r="B21" t="s">
+      <c r="E21" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="b">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="b">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="b">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="b">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="b">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="b">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="b">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B37" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B38" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B39" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="C61" s="4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C62" s="6">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>7</v>
+      </c>
+      <c r="B65" t="s">
+        <v>9</v>
+      </c>
+      <c r="C65" t="s">
+        <v>8</v>
+      </c>
+      <c r="D65" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66">
+        <v>0.75</v>
+      </c>
+      <c r="C66">
+        <v>0.2</v>
+      </c>
+      <c r="D66">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>6</v>
+      </c>
+      <c r="B67">
+        <v>0.15</v>
+      </c>
+      <c r="C67">
+        <v>0.35</v>
+      </c>
+      <c r="D67">
         <v>0.5</v>
       </c>
-      <c r="B22">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>3</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B71">
+        <v>0.7</v>
+      </c>
+      <c r="C71">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>6</v>
+      </c>
+      <c r="B72">
+        <v>0.4</v>
+      </c>
+      <c r="C72">
         <v>0.6</v>
       </c>
-      <c r="C26" s="4">
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>19</v>
+      </c>
+      <c r="B75" t="s">
+        <v>20</v>
+      </c>
+      <c r="C75" t="s">
+        <v>21</v>
+      </c>
+      <c r="D75" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>5</v>
+      </c>
+      <c r="B76">
+        <v>0.1</v>
+      </c>
+      <c r="C76">
+        <v>0.2</v>
+      </c>
+      <c r="D76">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>6</v>
+      </c>
+      <c r="B77">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="C27" s="6">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C30" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31">
-        <v>0.75</v>
-      </c>
-      <c r="C31">
-        <v>0.2</v>
-      </c>
-      <c r="D31">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32">
-        <v>0.15</v>
-      </c>
-      <c r="C32">
-        <v>0.35</v>
-      </c>
-      <c r="D32">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>3</v>
-      </c>
-      <c r="B35" t="s">
-        <v>1</v>
-      </c>
-      <c r="C35" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36">
-        <v>0.7</v>
-      </c>
-      <c r="C36">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37">
+      <c r="C77">
         <v>0.4</v>
       </c>
-      <c r="C37">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>19</v>
-      </c>
-      <c r="B40" t="s">
-        <v>20</v>
-      </c>
-      <c r="C40" t="s">
-        <v>21</v>
-      </c>
-      <c r="D40" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>5</v>
-      </c>
-      <c r="B41">
-        <v>0.1</v>
-      </c>
-      <c r="C41">
-        <v>0.2</v>
-      </c>
-      <c r="D41">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>6</v>
-      </c>
-      <c r="B42">
-        <v>0.4</v>
-      </c>
-      <c r="C42">
-        <v>0.4</v>
-      </c>
-      <c r="D42">
+      <c r="D77">
         <v>0.2</v>
       </c>
     </row>
@@ -998,7 +1268,7 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="7">
+  <tableParts count="8">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -1006,6 +1276,7 @@
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add cpt for timesteps and update mk_dbn
</commit_message>
<xml_diff>
--- a/CPTs.xlsx
+++ b/CPTs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rylan\Desktop\School\3Year\COSC329\329-Learning-Calendar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857F9296-7E8C-46D4-A496-28512B6E75A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{862F4168-8F85-4ACB-A123-5BB42EC0FA2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-8235" windowWidth="16440" windowHeight="28440" xr2:uid="{4FD7F259-FAFA-4789-A3F8-7C8F0A1F6558}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4FD7F259-FAFA-4789-A3F8-7C8F0A1F6558}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="36">
   <si>
     <t>EventImportance</t>
   </si>
@@ -133,6 +133,15 @@
   </si>
   <si>
     <t>Pr(WithinMonth)</t>
+  </si>
+  <si>
+    <t>NeedReminder_t-1</t>
+  </si>
+  <si>
+    <t>pr(NeedReminder_t | NeedReminder_t-1)</t>
+  </si>
+  <si>
+    <t>pr(~NeedReminder_t | NeedReminder_t-1)</t>
   </si>
 </sst>
 </file>
@@ -757,17 +766,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F16022FB-2605-4D33-9734-5034D9D67958}">
-  <dimension ref="A2:E47"/>
+  <dimension ref="A2:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="39.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
@@ -1272,6 +1280,39 @@
       </c>
       <c r="C47">
         <v>0.1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>33</v>
+      </c>
+      <c r="B50" t="s">
+        <v>35</v>
+      </c>
+      <c r="C50" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="b">
+        <v>0</v>
+      </c>
+      <c r="B51">
+        <v>0.65</v>
+      </c>
+      <c r="C51">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="b">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>0.1</v>
+      </c>
+      <c r="C52">
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make CPT for Needreminder_t
</commit_message>
<xml_diff>
--- a/CPTs.xlsx
+++ b/CPTs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rylan\Desktop\School\3Year\COSC329\329-Learning-Calendar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3084477B-47FE-4F01-98B1-495D28F0F82A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49108847-B42C-4B0E-855B-895E78C24C12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4FD7F259-FAFA-4789-A3F8-7C8F0A1F6558}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="39">
   <si>
     <t>EventImportance</t>
   </si>
@@ -142,6 +142,15 @@
   </si>
   <si>
     <t>Pr(FarAway|Urgent)2</t>
+  </si>
+  <si>
+    <t>Urgency_t</t>
+  </si>
+  <si>
+    <t>pr(~NR_t | NR_t-1 URG BUSY CCF)</t>
+  </si>
+  <si>
+    <t>pr(NR_t | NR_t-1 URG BUSY CCF)</t>
   </si>
 </sst>
 </file>
@@ -206,7 +215,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -255,6 +264,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -343,15 +358,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -364,9 +380,11 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="6"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="6" builtinId="32"/>
     <cellStyle name="Accent6" xfId="5" builtinId="49"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -800,20 +818,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F16022FB-2605-4D33-9734-5034D9D67958}">
-  <dimension ref="A2:F72"/>
+  <dimension ref="A2:G111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.5703125" customWidth="1"/>
-    <col min="3" max="3" width="40.5703125" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1531,13 +1549,13 @@
         <v>21</v>
       </c>
       <c r="E64">
-        <v>0.85</v>
+        <v>0.75</v>
       </c>
       <c r="F64">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B65" s="7" t="b">
         <v>1</v>
       </c>
@@ -1554,7 +1572,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B66" s="7" t="b">
         <v>1</v>
       </c>
@@ -1565,13 +1583,13 @@
         <v>19</v>
       </c>
       <c r="E66">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="F66">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67" s="7" t="b">
         <v>1</v>
       </c>
@@ -1582,13 +1600,13 @@
         <v>21</v>
       </c>
       <c r="E67" s="11">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="F67" s="11">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B68" s="7" t="b">
         <v>1</v>
       </c>
@@ -1599,13 +1617,13 @@
         <v>20</v>
       </c>
       <c r="E68" s="11">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="F68" s="11">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B69" s="7" t="b">
         <v>1</v>
       </c>
@@ -1622,7 +1640,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B70" s="7" t="b">
         <v>1</v>
       </c>
@@ -1633,13 +1651,13 @@
         <v>21</v>
       </c>
       <c r="E70">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="F70">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B71" s="7" t="b">
         <v>1</v>
       </c>
@@ -1656,7 +1674,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B72" s="7" t="b">
         <v>1</v>
       </c>
@@ -1671,6 +1689,782 @@
       </c>
       <c r="F72">
         <v>0.95</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B75" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C75" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D75" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F75" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G75" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B76" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C76" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E76" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F76">
+        <v>0.98</v>
+      </c>
+      <c r="G76">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B77" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C77" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F77">
+        <v>0.95</v>
+      </c>
+      <c r="G77">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B78" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C78" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E78" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F78">
+        <v>0.93</v>
+      </c>
+      <c r="G78">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B79" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C79" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D79" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E79" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F79" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="G79" s="12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B80" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C80" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D80" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F80" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="G80" s="12">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B81" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C81" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D81" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F81" s="12">
+        <v>0.85</v>
+      </c>
+      <c r="G81" s="12">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B82" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C82" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E82" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F82">
+        <v>0.85</v>
+      </c>
+      <c r="G82">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B83" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C83" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D83" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E83" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F83">
+        <v>0.8</v>
+      </c>
+      <c r="G83">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B84" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C84" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D84" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E84" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F84">
+        <v>0.75</v>
+      </c>
+      <c r="G84">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B85" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C85" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D85" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E85" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F85" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="G85" s="12">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B86" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C86" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D86" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E86" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F86" s="12">
+        <v>0.6</v>
+      </c>
+      <c r="G86" s="12">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B87" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C87" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E87" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F87" s="12">
+        <v>0.35</v>
+      </c>
+      <c r="G87" s="12">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B88" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C88" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D88" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E88" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F88">
+        <v>0.75</v>
+      </c>
+      <c r="G88">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B89" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C89" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D89" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F89">
+        <v>0.4</v>
+      </c>
+      <c r="G89">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B90" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C90" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D90" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E90" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F90">
+        <v>0.3</v>
+      </c>
+      <c r="G90">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B91" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C91" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E91" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F91" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="G91" s="12">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B92" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C92" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E92" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F92" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="G92" s="12">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B93" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C93" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E93" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F93" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="G93" s="12">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B94" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C94" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D94" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E94" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F94">
+        <f xml:space="preserve"> G93</f>
+        <v>0.95</v>
+      </c>
+      <c r="G94">
+        <f>F93</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B95" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C95" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D95" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E95" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F95">
+        <f xml:space="preserve"> G92</f>
+        <v>0.8</v>
+      </c>
+      <c r="G95">
+        <f xml:space="preserve"> F92</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B96" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C96" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E96" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F96">
+        <f xml:space="preserve"> G91</f>
+        <v>0.6</v>
+      </c>
+      <c r="G96">
+        <f xml:space="preserve"> F91</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B97" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C97" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D97" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E97" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F97" s="12">
+        <f xml:space="preserve"> G90</f>
+        <v>0.7</v>
+      </c>
+      <c r="G97" s="12">
+        <f xml:space="preserve"> F90</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B98" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C98" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D98" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E98" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F98" s="12">
+        <f xml:space="preserve"> G89</f>
+        <v>0.6</v>
+      </c>
+      <c r="G98" s="12">
+        <f xml:space="preserve"> F89</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B99" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C99" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D99" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E99" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F99" s="12">
+        <f xml:space="preserve"> G88</f>
+        <v>0.25</v>
+      </c>
+      <c r="G99" s="12">
+        <f xml:space="preserve"> F88</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B100" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C100" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D100" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E100" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F100">
+        <f xml:space="preserve"> G87</f>
+        <v>0.65</v>
+      </c>
+      <c r="G100">
+        <f>F87</f>
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B101" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C101" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D101" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E101" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F101">
+        <f xml:space="preserve"> G86</f>
+        <v>0.4</v>
+      </c>
+      <c r="G101">
+        <f>F86</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B102" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C102" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D102" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E102" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F102">
+        <f xml:space="preserve"> G85</f>
+        <v>0.2</v>
+      </c>
+      <c r="G102">
+        <f xml:space="preserve"> F85</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B103" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C103" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D103" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E103" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F103" s="12">
+        <f xml:space="preserve"> G84</f>
+        <v>0.25</v>
+      </c>
+      <c r="G103" s="12">
+        <f xml:space="preserve"> F84</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B104" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C104" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D104" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E104" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F104" s="12">
+        <f xml:space="preserve"> G83</f>
+        <v>0.2</v>
+      </c>
+      <c r="G104" s="12">
+        <f>F83</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B105" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C105" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D105" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E105" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F105" s="12">
+        <f xml:space="preserve"> G82</f>
+        <v>0.15</v>
+      </c>
+      <c r="G105" s="12">
+        <f xml:space="preserve"> F82</f>
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B106" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C106" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D106" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E106" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F106">
+        <f xml:space="preserve"> G81</f>
+        <v>0.15</v>
+      </c>
+      <c r="G106">
+        <f>F81</f>
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B107" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C107" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D107" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E107" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F107">
+        <f xml:space="preserve"> G80</f>
+        <v>0.1</v>
+      </c>
+      <c r="G107">
+        <f xml:space="preserve"> F80</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B108" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C108" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D108" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E108" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F108">
+        <f xml:space="preserve"> G79</f>
+        <v>0.05</v>
+      </c>
+      <c r="G108">
+        <f xml:space="preserve"> F79</f>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B109" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C109" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D109" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E109" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F109" s="12">
+        <f xml:space="preserve"> G78</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G109" s="12">
+        <f xml:space="preserve"> F78</f>
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B110" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C110" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D110" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E110" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F110" s="12">
+        <f xml:space="preserve"> G77</f>
+        <v>0.05</v>
+      </c>
+      <c r="G110" s="12">
+        <f xml:space="preserve"> F77</f>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B111" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C111" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D111" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E111" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F111" s="12">
+        <f xml:space="preserve"> G76</f>
+        <v>0.02</v>
+      </c>
+      <c r="G111" s="12">
+        <f>F76</f>
+        <v>0.98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>